<commit_message>
Recommit binary files to fix line endings
</commit_message>
<xml_diff>
--- a/Chlamydia/data/2016/CT notifications_2016_National_Estimate.xlsx
+++ b/Chlamydia/data/2016/CT notifications_2016_National_Estimate.xlsx
@@ -6559,8 +6559,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE67EE9C3B32F24C997F08FEDABFE4D4" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1916f590a0ac81e522d2d2b1bccf56e5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d22f42-674e-4fc3-9806-bf5045c6d197" xmlns:ns3="32705bbd-d6e6-412c-a7e2-7411e947c69b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d3581f47fd99f84d882c8689db76efb4" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE67EE9C3B32F24C997F08FEDABFE4D4" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60c22afda614b97921dbb231d6f04942">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d22f42-674e-4fc3-9806-bf5045c6d197" xmlns:ns3="32705bbd-d6e6-412c-a7e2-7411e947c69b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87248bdc6f4646256e6432bc260be0e0" ns2:_="" ns3:_="">
     <xsd:import namespace="e2d22f42-674e-4fc3-9806-bf5045c6d197"/>
     <xsd:import namespace="32705bbd-d6e6-412c-a7e2-7411e947c69b"/>
     <xsd:element name="properties">
@@ -6579,6 +6579,8 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6629,6 +6631,18 @@
     <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -6777,7 +6791,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBC923D4-EB41-49A5-9C3A-2CB33ADA9258}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{422676E4-0DD5-4201-AA8E-AC0CB0F28BB6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>